<commit_message>
affichage des epub de la db
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_PhilippeHeijkoop.xlsx
+++ b/Journal-de-Travail_PhilippeHeijkoop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pf25xeu\Documents\GitHub\P_AppMobile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1DA8D0-40C4-4D5F-B8A3-BCE0EDF728A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B38CC3-8D10-48CF-B210-4882CC7BCA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -163,6 +163,36 @@
   </si>
   <si>
     <t>J'ai refait la db, j'ai essayer d'afficher le epub de la db dans l'application mais je n'arrive pas a l'afficher et à l'enregistrer dans le téléphone</t>
+  </si>
+  <si>
+    <t>Séance des délégués</t>
+  </si>
+  <si>
+    <t>Problème http</t>
+  </si>
+  <si>
+    <t>J'ai réussi à lire l'EPUB depuis la requete http et afficher le contenu mais ce n'est pas parfait</t>
+  </si>
+  <si>
+    <t>Les informations sont coupées parce que le scrollView ne marche pas</t>
+  </si>
+  <si>
+    <t>Adapation du Backend pour insérer tout les epub dans la db</t>
+  </si>
+  <si>
+    <t>Route par ID pour récupérer les livres</t>
+  </si>
+  <si>
+    <t>C'est impossible d'envoyer plusieurs fichiers avec un res.send()</t>
+  </si>
+  <si>
+    <t>J'affiche le titre de tout les epub de la DB</t>
+  </si>
+  <si>
+    <t>TODO faire une route qui retourne le nombre de fichier présent pour connaitre le nombre de livre à récupérer</t>
+  </si>
+  <si>
+    <t>14h17</t>
   </si>
 </sst>
 </file>
@@ -1068,10 +1098,10 @@
                   <c:v>4.1666666666666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.50347222222222221</c:v>
+                  <c:v>0.55555555555555558</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2.7777777777777776E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1998,8 +2028,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <pane ySplit="6" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2052,7 +2082,7 @@
       </c>
       <c r="C3" s="25" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 13 heurs 15 minutes</v>
+        <v>0 jours 15 heurs 9 minutes</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="3"/>
@@ -2071,11 +2101,11 @@
       </c>
       <c r="D4" s="25">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>255</v>
+        <v>370</v>
       </c>
       <c r="E4" s="52">
         <f>SUM(C4:D4)</f>
-        <v>795</v>
+        <v>910</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2485,14 +2515,18 @@
       <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="str">
+      <c r="A22" s="8">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="39"/>
+        <v>18</v>
+      </c>
+      <c r="B22" s="39">
+        <v>45411</v>
+      </c>
       <c r="C22" s="35"/>
       <c r="D22" s="43"/>
-      <c r="F22" s="48"/>
+      <c r="F22" s="48" t="s">
+        <v>41</v>
+      </c>
       <c r="G22" s="17"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -2508,14 +2542,23 @@
       <c r="G23" s="20"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="str">
+      <c r="A24" s="8">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="39"/>
+        <v>19</v>
+      </c>
+      <c r="B24" s="39">
+        <v>45418</v>
+      </c>
       <c r="C24" s="35"/>
-      <c r="D24" s="43"/>
-      <c r="F24" s="48"/>
+      <c r="D24" s="43">
+        <v>40</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="48" t="s">
+        <v>42</v>
+      </c>
       <c r="G24" s="17"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -2525,10 +2568,18 @@
       </c>
       <c r="B25" s="40"/>
       <c r="C25" s="36"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="20"/>
+      <c r="D25" s="44">
+        <v>20</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="str">
@@ -2537,8 +2588,15 @@
       </c>
       <c r="B26" s="39"/>
       <c r="C26" s="35"/>
-      <c r="D26" s="43"/>
-      <c r="F26" s="48"/>
+      <c r="D26" s="43">
+        <v>20</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="48" t="s">
+        <v>45</v>
+      </c>
       <c r="G26" s="17"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -2548,21 +2606,38 @@
       </c>
       <c r="B27" s="40"/>
       <c r="C27" s="36"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="20"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D27" s="44">
+        <v>25</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="str">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
         <v/>
       </c>
       <c r="B28" s="39"/>
       <c r="C28" s="35"/>
-      <c r="D28" s="43"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="17"/>
+      <c r="D28" s="43">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="str">
@@ -2573,7 +2648,9 @@
       <c r="C29" s="36"/>
       <c r="D29" s="44"/>
       <c r="E29" s="19"/>
-      <c r="F29" s="47"/>
+      <c r="F29" s="47" t="s">
+        <v>50</v>
+      </c>
       <c r="G29" s="20"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -8467,7 +8544,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>245</v>
+        <v>320</v>
       </c>
       <c r="C5" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8475,7 +8552,7 @@
       </c>
       <c r="D5" s="45">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.50347222222222221</v>
+        <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8485,7 +8562,7 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C6" s="29" t="str">
         <f>'Journal de travail'!M10</f>
@@ -8493,7 +8570,7 @@
       </c>
       <c r="D6" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.7777777777777776E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -8584,7 +8661,7 @@
       </c>
       <c r="D12" s="46">
         <f>SUM(D4:D11)</f>
-        <v>0.55208333333333326</v>
+        <v>0.63194444444444442</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8606,18 +8683,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="19" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f3418dd4ca302601ba73fa17965a3f21">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns4="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5d82fd028d299635ce1df2d808d1b2ae" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -8883,6 +8948,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -8892,20 +8969,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2AC923F-FD8C-4D8C-BC85-CA1561E8B39C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8923,4 +8986,18 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update app, affichage des livre avec cover
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_PhilippeHeijkoop.xlsx
+++ b/Journal-de-Travail_PhilippeHeijkoop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pf25xeu\Documents\GitHub\P_AppMobile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B38CC3-8D10-48CF-B210-4882CC7BCA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104D0AF6-EA77-435E-85D4-3DFD9B22265D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -192,7 +192,10 @@
     <t>TODO faire une route qui retourne le nombre de fichier présent pour connaitre le nombre de livre à récupérer</t>
   </si>
   <si>
-    <t>14h17</t>
+    <t>Aide pour Adrian</t>
+  </si>
+  <si>
+    <t>Affichage de la cover du livre</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1101,7 @@
                   <c:v>4.1666666666666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.55555555555555558</c:v>
+                  <c:v>0.57986111111111116</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.7777777777777776E-2</c:v>
@@ -2028,8 +2031,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2082,7 +2085,7 @@
       </c>
       <c r="C3" s="25" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 15 heurs 9 minutes</v>
+        <v>0 jours 15 heurs 45 minutes</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="3"/>
@@ -2101,11 +2104,11 @@
       </c>
       <c r="D4" s="25">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>370</v>
+        <v>405</v>
       </c>
       <c r="E4" s="52">
         <f>SUM(C4:D4)</f>
-        <v>910</v>
+        <v>945</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2648,9 +2651,7 @@
       <c r="C29" s="36"/>
       <c r="D29" s="44"/>
       <c r="E29" s="19"/>
-      <c r="F29" s="47" t="s">
-        <v>50</v>
-      </c>
+      <c r="F29" s="47"/>
       <c r="G29" s="20"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -2660,8 +2661,15 @@
       </c>
       <c r="B30" s="39"/>
       <c r="C30" s="35"/>
-      <c r="D30" s="43"/>
-      <c r="F30" s="48"/>
+      <c r="D30" s="43">
+        <v>25</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="48" t="s">
+        <v>50</v>
+      </c>
       <c r="G30" s="17"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -2671,9 +2679,15 @@
       </c>
       <c r="B31" s="40"/>
       <c r="C31" s="36"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="47"/>
+      <c r="D31" s="44">
+        <v>10</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="47" t="s">
+        <v>51</v>
+      </c>
       <c r="G31" s="20"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -8544,7 +8558,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>320</v>
+        <v>355</v>
       </c>
       <c r="C5" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8552,7 +8566,7 @@
       </c>
       <c r="D5" s="45">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.55555555555555558</v>
+        <v>0.57986111111111116</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8661,7 +8675,7 @@
       </c>
       <c r="D12" s="46">
         <f>SUM(D4:D11)</f>
-        <v>0.63194444444444442</v>
+        <v>0.65625</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8683,6 +8697,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="19" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f3418dd4ca302601ba73fa17965a3f21">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns4="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5d82fd028d299635ce1df2d808d1b2ae" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -8948,18 +8974,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -8969,6 +8983,20 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2AC923F-FD8C-4D8C-BC85-CA1561E8B39C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8986,18 +9014,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>